<commit_message>
almost done w/ schematic, just need to finish footprint assignment (make sure buck converter components are correctly chosen and there aren't caps that need to be different and stuff)
</commit_message>
<xml_diff>
--- a/BuckCalcs.xlsx
+++ b/BuckCalcs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="20-&gt;12" sheetId="1" state="visible" r:id="rId1"/>
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -214,7 +214,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,9 +238,9 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>452437</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>112920</xdr:rowOff>
+      <xdr:rowOff>112919</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2539998" cy="922547"/>
+    <xdr:ext cx="2539997" cy="922547"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="184882162" name=""/>
@@ -301,7 +300,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>404812</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>128795</xdr:rowOff>
+      <xdr:rowOff>128794</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2333624" cy="639348"/>
     <xdr:pic>
@@ -1014,7 +1013,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1259,7 +1258,7 @@
         <v>29</v>
       </c>
       <c r="D26">
-        <f>D23+D22/2</f>
+        <f>B24+D22</f>
         <v>12.142857142857142</v>
       </c>
     </row>
@@ -1315,7 +1314,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" id="{00F200D5-002D-448D-B4B7-008900210020}">
+          <x14:cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" id="{006C00AA-0008-4162-916E-00D30013007B}">
             <xm:f>5.5</xm:f>
             <x14:dxf>
               <font>
@@ -1332,7 +1331,7 @@
           <xm:sqref>D13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="lessThan" id="{007E00DD-00B4-4936-9650-000500B800B0}">
+          <x14:cfRule type="cellIs" priority="1" operator="lessThan" id="{00D60026-00C2-4657-BF54-006700B80036}">
             <xm:f>5.5</xm:f>
             <x14:dxf>
               <font>
@@ -1408,10 +1407,10 @@
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>850000</v>
       </c>
     </row>
@@ -1435,7 +1434,7 @@
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B10">

</xml_diff>

<commit_message>
finished addressing review comments & organized bom with p/ns for everything
</commit_message>
<xml_diff>
--- a/BuckCalcs.xlsx
+++ b/BuckCalcs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="20-&gt;12" sheetId="1" state="visible" r:id="rId1"/>
@@ -1314,7 +1314,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" id="{006C00AA-0008-4162-916E-00D30013007B}">
+          <x14:cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" id="{008D0016-0023-4393-88B7-001B0018005F}">
             <xm:f>5.5</xm:f>
             <x14:dxf>
               <font>
@@ -1331,7 +1331,7 @@
           <xm:sqref>D13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="lessThan" id="{00D60026-00C2-4657-BF54-006700B80036}">
+          <x14:cfRule type="cellIs" priority="1" operator="lessThan" id="{0076003D-00AD-4C85-BBD3-00CA00F8008E}">
             <xm:f>5.5</xm:f>
             <x14:dxf>
               <font>
@@ -1403,7 +1403,7 @@
         <v>25</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B11">
         <f>B5+B10/2</f>
-        <v>2.5199049316696378</v>
+        <v>3.0199049316696378</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="B12">
         <f>SQRT(B5^2+(1/12)*B10^2)</f>
-        <v>2.0223996586542441</v>
+        <v>2.5179555951852692</v>
       </c>
       <c r="E12" s="3"/>
     </row>

</xml_diff>

<commit_message>
Addressed most of the review comments, fixed power protection, added bigger caps & better part selection on 12V and 5V out, changed 5V buck inductor, fixed power good & fault LEDs
</commit_message>
<xml_diff>
--- a/BuckCalcs.xlsx
+++ b/BuckCalcs.xlsx
@@ -1314,7 +1314,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" id="{008D0016-0023-4393-88B7-001B0018005F}">
+          <x14:cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" id="{007900E4-0087-44BA-9829-00F3002100DC}">
             <xm:f>5.5</xm:f>
             <x14:dxf>
               <font>
@@ -1331,7 +1331,7 @@
           <xm:sqref>D13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="lessThan" id="{0076003D-00AD-4C85-BBD3-00CA00F8008E}">
+          <x14:cfRule type="cellIs" priority="1" operator="lessThan" id="{00B2008D-003C-4865-A3D5-00DD00D200A9}">
             <xm:f>5.5</xm:f>
             <x14:dxf>
               <font>
@@ -1429,8 +1429,8 @@
         <v>36</v>
       </c>
       <c r="B9">
-        <f>3.3*10^-6</f>
-        <v>3.2999999999999997e-06</v>
+        <f>4.7*10^-6</f>
+        <v>4.6999999999999999e-06</v>
       </c>
     </row>
     <row r="10" ht="14.25">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B10">
         <f>B4/B3*(B3-B4)/(B9*B6)</f>
-        <v>1.0398098633392754</v>
+        <v>0.73007926574885273</v>
       </c>
       <c r="E10" s="5"/>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="B11">
         <f>B5+B10/2</f>
-        <v>3.0199049316696378</v>
+        <v>2.8650396328744265</v>
       </c>
       <c r="E11" s="4"/>
     </row>
@@ -1459,7 +1459,7 @@
       </c>
       <c r="B12">
         <f>SQRT(B5^2+(1/12)*B10^2)</f>
-        <v>2.5179555951852692</v>
+        <v>2.5088678677555669</v>
       </c>
       <c r="E12" s="3"/>
     </row>

</xml_diff>